<commit_message>
Added All the code in the dev
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\SeleniumFremwork\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC75086-5503-4E12-8534-42BAE091AB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EE8ADB-2BFB-46E8-B0E1-6BCC411E5B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BBC49AF1-C3D1-4265-BD12-E7810C125702}"/>
   </bookViews>
   <sheets>
-    <sheet name="Testdata" sheetId="1" r:id="rId1"/>
+    <sheet name="Testdata" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -429,11 +429,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10FFEE68-2473-4DE3-A7FE-6087EEB5BC9E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B940C723-A2F7-4E70-9B32-144EB07FD5B9}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +459,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{B4EE16A0-7456-4F03-8474-34B12E3A24F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>